<commit_message>
Released expander magnetic encoder and updated expander breakout.
</commit_message>
<xml_diff>
--- a/PCB modules/magnetic encoder/harp expander magnetic encoder v1.0 BOM.xlsx
+++ b/PCB modules/magnetic encoder/harp expander magnetic encoder v1.0 BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_expander\PCB modules\magnetic encoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FA8912-D321-44D2-9E67-B814C0E7A510}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B40613-9DED-4FA5-9004-E47D3BD9C03D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22DE42AE-D7DB-44FC-B9CF-DE1961A005DB}"/>
   </bookViews>
@@ -152,12 +152,6 @@
     <t>C1, C2, C3</t>
   </si>
   <si>
-    <t>TLV70033DDCR</t>
-  </si>
-  <si>
-    <t>296-27937-6-ND</t>
-  </si>
-  <si>
     <t>10uF 16V X5R 20%</t>
   </si>
   <si>
@@ -176,9 +170,6 @@
     <t>SOT-23-5</t>
   </si>
   <si>
-    <t>LDO 3.3V 200mA</t>
-  </si>
-  <si>
     <t>SN74LVC1G125DBVT</t>
   </si>
   <si>
@@ -216,6 +207,15 @@
   </si>
   <si>
     <t>AKC10H-ND</t>
+  </si>
+  <si>
+    <t>LP5907MFX-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>296-38557-6-ND</t>
+  </si>
+  <si>
+    <t>Ultra-Low-Noise LDO 3.3V 250mA</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1143,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1201,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -1219,7 +1219,7 @@
         <v>27</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1227,7 +1227,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>20</v>
@@ -1245,7 +1245,7 @@
         <v>27</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1253,16 +1253,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>10</v>
@@ -1271,7 +1271,7 @@
         <v>27</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1279,16 +1279,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>10</v>
@@ -1297,24 +1297,24 @@
         <v>27</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>1</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>40</v>
+      <c r="B7" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>10</v>
@@ -1322,8 +1322,8 @@
       <c r="G7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>33</v>
+      <c r="H7" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1377,13 +1377,13 @@
         <v>16</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1394,16 +1394,16 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I11" t="s">
         <v>28</v>

</xml_diff>